<commit_message>
Milestone Report Drafted/ fixed naming conventions of files
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CD57B0-38E5-4894-A0F2-5C1FA5246F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F5816-3E0B-479B-B5EC-37DB70D6C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <t>Week:</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Edited Git README</t>
+  </si>
+  <si>
+    <t>Milestone #1 report</t>
+  </si>
+  <si>
+    <t>Fixed naming conventions of files, added warning to README due to the likelihood of the the repo going public</t>
   </si>
 </sst>
 </file>
@@ -1522,10 +1528,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1650</c:v>
+                  <c:v>1740</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7050</c:v>
+                  <c:v>6960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10524,7 +10530,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10840,16 +10846,32 @@
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="24"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="C23" s="32">
+        <v>45946</v>
+      </c>
+      <c r="D23" s="22">
+        <v>75</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="25"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="C24" s="33">
+        <v>45946</v>
+      </c>
+      <c r="D24" s="23">
+        <v>15</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25" s="24"/>
@@ -16762,11 +16784,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>1650</v>
+        <v>1740</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>7050</v>
+        <v>6960</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Home Page information
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F5816-3E0B-479B-B5EC-37DB70D6C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8B697D-740B-442D-B989-9FC05653C6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Week:</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Fixed naming conventions of files, added warning to README due to the likelihood of the the repo going public</t>
+  </si>
+  <si>
+    <t>Standup log and MISC documentation</t>
   </si>
 </sst>
 </file>
@@ -1528,10 +1531,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1740</c:v>
+                  <c:v>1770</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6960</c:v>
+                  <c:v>6930</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10125,7 +10128,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10530,7 +10533,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10874,10 +10877,18 @@
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="24"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
+      <c r="C25" s="32">
+        <v>45946</v>
+      </c>
+      <c r="D25" s="22">
+        <v>30</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="25"/>
@@ -16784,11 +16795,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>1740</v>
+        <v>1770</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>6960</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Week 4 Standup Submitted
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6793D9BE-F502-45ED-8817-B4486A86A18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E37401-327A-4922-94E1-7E61F1A005D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -10536,7 +10536,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E30" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Milestone 1 Report Final
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E37401-327A-4922-94E1-7E61F1A005D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B69E9A9-1ED6-4B16-9ECB-209F2F955D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Week:</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Finsihing up starter storboards</t>
+  </si>
+  <si>
+    <t>Finalized presentation and Milestone 1 report</t>
   </si>
 </sst>
 </file>
@@ -1534,10 +1537,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1920</c:v>
+                  <c:v>1980</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6780</c:v>
+                  <c:v>6720</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10536,7 +10539,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E29:E30"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10922,10 +10925,18 @@
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="25"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="C28" s="33">
+        <v>45946</v>
+      </c>
+      <c r="D28" s="23">
+        <v>60</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" s="24"/>
@@ -16814,11 +16825,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>1920</v>
+        <v>1980</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>6780</v>
+        <v>6720</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Base Dev Env. Created
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B69E9A9-1ED6-4B16-9ECB-209F2F955D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CFBCAC-71AC-418D-91ED-70050505B797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="43035" yWindow="3570" windowWidth="14745" windowHeight="7470" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Week:</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Finalized presentation and Milestone 1 report</t>
+  </si>
+  <si>
+    <t>Dev Env. Stood up</t>
+  </si>
+  <si>
+    <t>Database outline created and implemented</t>
   </si>
 </sst>
 </file>
@@ -1537,10 +1543,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1980</c:v>
+                  <c:v>2175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6720</c:v>
+                  <c:v>6525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10539,7 +10545,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F1" activeCellId="1" sqref="F33 F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10939,16 +10945,32 @@
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="24"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
+      <c r="C29" s="32">
+        <v>45950</v>
+      </c>
+      <c r="D29" s="22">
+        <v>90</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="25"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="C30" s="33">
+        <v>45950</v>
+      </c>
+      <c r="D30" s="23">
+        <v>105</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C31" s="24"/>
@@ -16825,11 +16847,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>1980</v>
+        <v>2175</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>6720</v>
+        <v>6525</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added CUI Types top database
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CFBCAC-71AC-418D-91ED-70050505B797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65B1410-57EB-436D-BA28-6FD64D53774C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43035" yWindow="3570" windowWidth="14745" windowHeight="7470" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>Week:</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Database outline created and implemented</t>
+  </si>
+  <si>
+    <t>Added CUI types</t>
   </si>
 </sst>
 </file>
@@ -1543,10 +1546,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2175</c:v>
+                  <c:v>2265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6525</c:v>
+                  <c:v>6435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10545,7 +10548,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" activeCellId="1" sqref="F33 F1:F1048576"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10973,10 +10976,18 @@
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="24"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
+      <c r="C31" s="32">
+        <v>45950</v>
+      </c>
+      <c r="D31" s="22">
+        <v>90</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C32" s="25"/>
@@ -16847,11 +16858,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>2175</v>
+        <v>2265</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>6525</v>
+        <v>6435</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Inital look of first question
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252769CF-0572-4F4F-8543-0ADB29D72A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCDF673-5A4A-45AF-BAA8-E78966DE3E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
   <si>
     <t>Week:</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Worked on home page</t>
+  </si>
+  <si>
+    <t>small fixes</t>
+  </si>
+  <si>
+    <t>Working on first question page</t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1564,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2850</c:v>
+                  <c:v>2985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5850</c:v>
+                  <c:v>5715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10560,7 +10566,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11072,16 +11078,32 @@
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="24"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
+      <c r="C37" s="32">
+        <v>45957</v>
+      </c>
+      <c r="D37" s="22">
+        <v>45</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="25"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
+      <c r="C38" s="33">
+        <v>45958</v>
+      </c>
+      <c r="D38" s="23">
+        <v>90</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C39" s="24"/>
@@ -16910,11 +16932,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>2850</v>
+        <v>2985</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>5850</v>
+        <v>5715</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Init first session vars
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCDF673-5A4A-45AF-BAA8-E78966DE3E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202B828-24ED-4F9F-B73C-F62B7513EB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -1564,10 +1564,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2985</c:v>
+                  <c:v>3015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5715</c:v>
+                  <c:v>5685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10566,7 +10566,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11096,7 +11096,7 @@
         <v>45958</v>
       </c>
       <c r="D38" s="23">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>27</v>
@@ -16932,11 +16932,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>2985</v>
+        <v>3015</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>5715</v>
+        <v>5685</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added IAAS and result page
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202B828-24ED-4F9F-B73C-F62B7513EB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FA42C0-7F58-4C33-BB4B-EDF640D45E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -1564,10 +1564,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3015</c:v>
+                  <c:v>3075</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5685</c:v>
+                  <c:v>5625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10566,7 +10566,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11096,7 +11096,7 @@
         <v>45958</v>
       </c>
       <c r="D38" s="23">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>27</v>
@@ -16932,11 +16932,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>3015</v>
+        <v>3075</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>5685</v>
+        <v>5625</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AC questions partially added
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58C0462-4214-42DE-8B83-64BD1D33A4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8CA29D-C177-4D79-A4E0-D4A726B71DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
   <si>
     <t>Week:</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Fixing laptop XAMPP</t>
+  </si>
+  <si>
+    <t>Working on assessment</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -644,7 +647,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1113,6 +1115,100 @@
           <a:effectLst/>
         </c:spPr>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="88000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="76000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="53000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="41000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1256,6 +1352,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-5C21-4687-90FD-2477E5A7EA45}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1273,6 +1374,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-5C21-4687-90FD-2477E5A7EA45}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1290,6 +1396,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-5C21-4687-90FD-2477E5A7EA45}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1307,6 +1418,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-5C21-4687-90FD-2477E5A7EA45}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -1324,6 +1440,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-5C21-4687-90FD-2477E5A7EA45}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -1341,6 +1462,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-5C21-4687-90FD-2477E5A7EA45}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1704,10 +1830,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3195</c:v>
+                  <c:v>3465</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5505</c:v>
+                  <c:v>5235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9443,7 +9569,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{542969FB-8A7D-470E-946B-17B5961CB080}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{542969FB-8A7D-470E-946B-17B5961CB080}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="A18:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
@@ -9928,7 +10054,7 @@
   <dataFields count="1">
     <dataField name="Sum of Time (Mins)" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="12">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -9994,6 +10120,78 @@
           </reference>
           <reference field="2" count="1" selected="0">
             <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
@@ -10683,7 +10881,7 @@
       <c r="A19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19">
         <v>390</v>
       </c>
     </row>
@@ -10691,7 +10889,7 @@
       <c r="A20" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20">
         <v>600</v>
       </c>
     </row>
@@ -10699,13 +10897,12 @@
       <c r="A21" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="47"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22">
         <v>360</v>
       </c>
     </row>
@@ -10713,7 +10910,7 @@
       <c r="A23" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B23">
         <v>285</v>
       </c>
     </row>
@@ -10721,7 +10918,7 @@
       <c r="A24" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B24">
         <v>225</v>
       </c>
     </row>
@@ -10729,7 +10926,7 @@
       <c r="A25" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="47">
+      <c r="B25">
         <v>60</v>
       </c>
     </row>
@@ -10737,7 +10934,7 @@
       <c r="A26" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="47">
+      <c r="B26">
         <v>60</v>
       </c>
     </row>
@@ -10745,7 +10942,7 @@
       <c r="A27" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="47">
+      <c r="B27">
         <v>90</v>
       </c>
     </row>
@@ -10753,7 +10950,7 @@
       <c r="A28" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B28">
         <v>195</v>
       </c>
     </row>
@@ -10761,7 +10958,7 @@
       <c r="A29" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="47">
+      <c r="B29">
         <v>930</v>
       </c>
     </row>
@@ -10769,7 +10966,7 @@
       <c r="A30" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="47">
+      <c r="B30">
         <v>3195</v>
       </c>
     </row>
@@ -10800,8 +10997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8154930E-2F36-41CB-8896-D63BC278B832}">
   <dimension ref="C1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11355,15 +11552,29 @@
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="25"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
+      <c r="C40" s="33">
+        <v>45960</v>
+      </c>
+      <c r="D40" s="23">
+        <v>150</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="24"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
+      <c r="C41" s="32">
+        <v>45961</v>
+      </c>
+      <c r="D41" s="22">
+        <v>120</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F41" s="22"/>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.3">
@@ -17175,11 +17386,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>3195</v>
+        <v>3465</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>5505</v>
+        <v>5235</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed style sheet refrence
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EB71D6-FFA9-4FCD-BACA-806F61237AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7990C72-1F06-485B-B425-3095A9C4104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="71">
   <si>
     <t>Week:</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Working on assessment</t>
+  </si>
+  <si>
+    <t>Creating an AWS account and putting the CMMC Fledge websit eon there (CSS does not work on asessment pages)</t>
   </si>
 </sst>
 </file>
@@ -1830,10 +1833,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3795</c:v>
+                  <c:v>3930</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4905</c:v>
+                  <c:v>4770</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10998,7 +11001,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11594,10 +11597,18 @@
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="24"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
+      <c r="C43" s="32">
+        <v>45962</v>
+      </c>
+      <c r="D43" s="22">
+        <v>135</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C44" s="25"/>
@@ -17396,11 +17407,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>3795</v>
+        <v>3930</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4905</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
CMMC Cert Type w CUI drafted
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D8BD2-8A04-4080-BD66-FC94F7016035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A341804C-C9EA-4DD7-9AB0-8157C4F55966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
   <si>
     <t>Week:</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>Creating an AWS account and putting the CMMC Fledge website on there (CSS does not work on asessment pages)</t>
+  </si>
+  <si>
+    <t>working on assessment</t>
+  </si>
+  <si>
+    <t>Fighting with CUI types</t>
   </si>
 </sst>
 </file>
@@ -1833,10 +1839,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3975</c:v>
+                  <c:v>4155</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4725</c:v>
+                  <c:v>4545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11001,7 +11007,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11615,18 +11621,28 @@
         <v>45963</v>
       </c>
       <c r="D44" s="23">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="23"/>
+      <c r="F44" s="23" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C45" s="24"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
+      <c r="C45" s="32">
+        <v>45963</v>
+      </c>
+      <c r="D45" s="22">
+        <v>135</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C46" s="25"/>
@@ -17413,11 +17429,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>3975</v>
+        <v>4155</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4725</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Focus set to CMMC L1 controls
Need to deliver the assessment report for Tuesday
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A341804C-C9EA-4DD7-9AB0-8157C4F55966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24198B16-83F2-403B-87A7-C3E2AA331A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -1839,10 +1839,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4155</c:v>
+                  <c:v>4185</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4545</c:v>
+                  <c:v>4515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11007,7 +11007,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11621,7 +11621,7 @@
         <v>45963</v>
       </c>
       <c r="D44" s="23">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>27</v>
@@ -17429,11 +17429,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4155</v>
+        <v>4185</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4545</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added l1 up to SC
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24198B16-83F2-403B-87A7-C3E2AA331A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512E66BB-BBFA-4158-BBD7-FA32E1FB467F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t>Week:</t>
   </si>
@@ -1839,10 +1839,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4185</c:v>
+                  <c:v>4215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4515</c:v>
+                  <c:v>4485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11007,7 +11007,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11645,10 +11645,18 @@
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C46" s="25"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
+      <c r="C46" s="33">
+        <v>45964</v>
+      </c>
+      <c r="D46" s="23">
+        <v>30</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C47" s="24"/>
@@ -17429,11 +17437,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4185</v>
+        <v>4215</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4515</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Question needed for initial report generation
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512E66BB-BBFA-4158-BBD7-FA32E1FB467F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106D02F2-7126-4490-BF8E-59F5F5999ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -1839,10 +1839,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4215</c:v>
+                  <c:v>4275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4485</c:v>
+                  <c:v>4425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11007,7 +11007,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11649,7 +11649,7 @@
         <v>45964</v>
       </c>
       <c r="D46" s="23">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E46" s="23" t="s">
         <v>27</v>
@@ -17437,11 +17437,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4215</v>
+        <v>4275</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4485</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SQL updated for l1
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106D02F2-7126-4490-BF8E-59F5F5999ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD79171E-6E83-4D60-9B42-2548449F1D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="70905" yWindow="3780" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>Week:</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>Fighting with CUI types</t>
+  </si>
+  <si>
+    <t>Working on assessment report for l1</t>
   </si>
 </sst>
 </file>
@@ -1839,10 +1842,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4275</c:v>
+                  <c:v>4335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4425</c:v>
+                  <c:v>4365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11006,8 +11009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8154930E-2F36-41CB-8896-D63BC278B832}">
   <dimension ref="C1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11659,10 +11662,18 @@
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C47" s="24"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
+      <c r="C47" s="32">
+        <v>45964</v>
+      </c>
+      <c r="D47" s="22">
+        <v>60</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C48" s="25"/>
@@ -17437,11 +17448,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4275</v>
+        <v>4335</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4425</v>
+        <v>4365</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Crazy switch statement added
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD79171E-6E83-4D60-9B42-2548449F1D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4121B7-C3F0-4221-B5F9-C68B211676D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="70905" yWindow="3780" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
   <si>
     <t>Week:</t>
   </si>
@@ -1842,10 +1842,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4335</c:v>
+                  <c:v>4395</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4365</c:v>
+                  <c:v>4305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11009,8 +11009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8154930E-2F36-41CB-8896-D63BC278B832}">
   <dimension ref="C1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11676,10 +11676,18 @@
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C48" s="25"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
+      <c r="C48" s="33">
+        <v>45965</v>
+      </c>
+      <c r="D48" s="23">
+        <v>60</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C49" s="24"/>
@@ -17448,11 +17456,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4335</v>
+        <v>4395</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4365</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
PE/ boundary report complete
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4121B7-C3F0-4221-B5F9-C68B211676D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3F0778-7520-45DA-A058-86A5A7504061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70905" yWindow="3780" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>Week:</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Working on assessment report for l1</t>
+  </si>
+  <si>
+    <t>Working on presentation for milestone 2</t>
   </si>
 </sst>
 </file>
@@ -1842,10 +1845,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4395</c:v>
+                  <c:v>4560</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4305</c:v>
+                  <c:v>4140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11010,7 +11013,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11680,7 +11683,7 @@
         <v>45965</v>
       </c>
       <c r="D48" s="23">
-        <v>60</v>
+        <v>195</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>27</v>
@@ -11690,10 +11693,18 @@
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C49" s="24"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
+      <c r="C49" s="32">
+        <v>45965</v>
+      </c>
+      <c r="D49" s="22">
+        <v>30</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C50" s="25"/>
@@ -17456,11 +17467,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4395</v>
+        <v>4560</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4305</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
CMMC L1 report ready
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762BFCA1-4149-4BB7-BBA3-340582AF96C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE79CB-266A-4464-A3F1-8DA7DDF921B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67080" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -1845,10 +1845,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4590</c:v>
+                  <c:v>4650</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4110</c:v>
+                  <c:v>4050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11013,7 +11013,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11683,7 +11683,7 @@
         <v>45965</v>
       </c>
       <c r="D48" s="23">
-        <v>225</v>
+        <v>285</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>27</v>
@@ -17467,11 +17467,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>4590</v>
+        <v>4650</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>4110</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
First touches with Dictionary page
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8A249E-AFF5-4FC3-ACE8-B124AAE18053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB6BFD2-803D-4E76-98E3-BBB5DA51A808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
+    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="85">
   <si>
     <t>Week:</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Changing website colors</t>
+  </si>
+  <si>
+    <t>fixing some styles, putting first touches on Fledge Dictonary</t>
   </si>
 </sst>
 </file>
@@ -1873,10 +1876,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5280</c:v>
+                  <c:v>5370</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3420</c:v>
+                  <c:v>3330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11041,7 +11044,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C42" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11854,17 +11857,25 @@
         <v>120</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F58" s="23" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C59" s="24"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
+      <c r="C59" s="32">
+        <v>45976</v>
+      </c>
+      <c r="D59" s="22">
+        <v>90</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C60" s="25"/>
@@ -17567,11 +17578,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>5280</v>
+        <v>5370</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>3420</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
About Us text added
</commit_message>
<xml_diff>
--- a/02_WorkingDocs/CMMCFledge_Workbook.xlsx
+++ b/02_WorkingDocs/CMMCFledge_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckm32\OneDrive\Desktop\CMMCFledge\02_WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB6BFD2-803D-4E76-98E3-BBB5DA51A808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9DF87D-8849-4B03-ADE1-A93759B2F021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{208106DA-3D21-4604-99AA-9AD5A5B6DE72}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>Week:</t>
   </si>
@@ -296,7 +296,10 @@
     <t>Changing website colors</t>
   </si>
   <si>
-    <t>fixing some styles, putting first touches on Fledge Dictonary</t>
+    <t>Discussion with outside stakeholder to discuss future look of result page and Dictonary page</t>
+  </si>
+  <si>
+    <t>fixing some styles, putting first touches on Fledge Dictonary, About us write up</t>
   </si>
 </sst>
 </file>
@@ -1876,10 +1879,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5370</c:v>
+                  <c:v>5490</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3330</c:v>
+                  <c:v>3210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11044,7 +11047,7 @@
   <dimension ref="C1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C42" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11868,20 +11871,28 @@
         <v>45976</v>
       </c>
       <c r="D59" s="22">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E59" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F59" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="33">
+        <v>45976</v>
+      </c>
+      <c r="D60" s="23">
+        <v>30</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="23" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C60" s="25"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C61" s="24"/>
@@ -17578,11 +17589,11 @@
       </c>
       <c r="D2">
         <f>SUM(Table2[Time (Mins)])</f>
-        <v>5370</v>
+        <v>5490</v>
       </c>
       <c r="E2">
         <f>8700-D2</f>
-        <v>3330</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>